<commit_message>
ZZZS doctors' availability data update 🤖
</commit_message>
<xml_diff>
--- a/zzzs/2023/05/2023-05-18_LokacijeZdrDelavcevOC.xlsx
+++ b/zzzs/2023/05/2023-05-18_LokacijeZdrDelavcevOC.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="Ta_delovni_zvezek"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EXCEL_AUTO_OSTALO\Porocila\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C893D2E9-E64D-4B82-9BFE-7807BCC42DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="73/1U22h4cplhPLfrvKtph7ZH5r5PALKuCv8x+L7xyFpA85AFObI2Epob1ZV0arSU12p3AN+9fbadytIF+foVg==" workbookSaltValue="IDYq/6iFGUg3Cm9FrTRjpQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{495C197E-1C8A-41A0-8E91-098E2FD3D7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="SD7zwixudMsbvCtPeiWQiJiTRnSL13i2TG0E2B42IHMetf/+G7U6hKGwqkeVfyGVCTlh76kRlVDzwiiZK4IMyg==" workbookSaltValue="W1tohZn7Xtg583GU9Vyypw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +40,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="odbc" type="1" refreshedVersion="8" deleted="1" saveData="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="odbc" type="1" refreshedVersion="7" deleted="1" saveData="1">
     <dbPr connection="" command=""/>
   </connection>
 </connections>
@@ -7632,7 +7630,7 @@
     <t>ŠMARTNO 70</t>
   </si>
   <si>
-    <t>Datum in čas priprave: 18.05.2023 11:06:54</t>
+    <t>Datum in èas priprave: 18.05.2023 13:01:50</t>
   </si>
 </sst>
 </file>
@@ -86641,7 +86639,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5+w3BGAu5Eof38ZkGJIygAhO5zyLnWSVoLeiCcxRodNbWBw0tNN0DP4+LN2kUJ7nGP+OQZUBe8QszyQufYl5DA==" saltValue="ihWORbU+t2Dm/X1hLe/vlQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wpjacoKcXN5E5fyN3pcmyAXow6DIeJGWjPHT1RAKT54Zs7GjxiGfUBVpjbN8a7skjUlQfc+TqvfFwUKS6F18/w==" saltValue="5vJtVNGL4ZOQ6g/ES3WiOw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="A4:C4"/>
   </mergeCells>

</xml_diff>